<commit_message>
Update phone merge logic and assets
</commit_message>
<xml_diff>
--- a/Tables/Org Chart and HUB 12-25.xlsx
+++ b/Tables/Org Chart and HUB 12-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Projects\uds-asset-management\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BDEEF6-5508-447A-AC95-0E5CD97F9313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD67040E-EEFA-4A29-B523-CD24CD832E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9B2D7EE0-D9D0-4145-AC80-0949B49CD4F5}"/>
   </bookViews>
@@ -3801,8 +3801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EED7661-F274-439F-B201-1B8FA64A435D}">
   <dimension ref="A1:N323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F73" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:XFD130"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>